<commit_message>
report_text function created. Not sure how to easily extract english text from spreadsheet
</commit_message>
<xml_diff>
--- a/Screener/Fundamental_Info.xlsx
+++ b/Screener/Fundamental_Info.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>Category</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Basic</t>
   </si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">Price to earnings is just one number to look at. High price to earnings can mean that the company is overvalued or it means that </t>
+  </si>
+  <si>
+    <t>justatest</t>
   </si>
 </sst>
 </file>
@@ -386,23 +386,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -410,49 +410,42 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>